<commit_message>
Works with multiple elements
</commit_message>
<xml_diff>
--- a/ifc_to_openroads/data/IFC.xlsx
+++ b/ifc_to_openroads/data/IFC.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <x:si>
     <x:t>Library</x:t>
   </x:si>
@@ -41,10 +41,19 @@
     <x:t>Default</x:t>
   </x:si>
   <x:si>
-    <x:t>73287</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0qcE4HvDG4HgitFiVRo11R</x:t>
+    <x:t>73366</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1hS$VweOwvHwyp3_HHdqTH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73368</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73369</x:t>
+  </x:si>
+  <x:si>
+    <x:t>73370</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -435,7 +444,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C2"/>
+  <x:dimension ref="A1:C5"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -443,7 +452,7 @@
   <x:cols>
     <x:col min="1" max="1" width="12.430625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="10.530625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="24.510625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="27.680625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
@@ -465,6 +474,39 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>

</xml_diff>